<commit_message>
Tela de controlar perfil e adição de historias para votação
</commit_message>
<xml_diff>
--- a/HistoriasProjetoRH.xlsx
+++ b/HistoriasProjetoRH.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yurim_000\Desktop\RH\prosperity\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7230"/>
   </bookViews>
   <sheets>
     <sheet name="Histórias" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="76">
   <si>
     <t>História</t>
   </si>
@@ -225,13 +220,40 @@
   </si>
   <si>
     <t>Verificar Jetty</t>
+  </si>
+  <si>
+    <t>Eu, ADM quero alterar status do usuário.</t>
+  </si>
+  <si>
+    <t>Eu, ADM quero acessar a tela de editar usuário</t>
+  </si>
+  <si>
+    <t>Eu, ADM quero redefinir senha do usuário</t>
+  </si>
+  <si>
+    <t>Eu, ADM quero salvar alterações no usuário</t>
+  </si>
+  <si>
+    <t>Eu, ADM quero acessar tela de Permissões de perfis</t>
+  </si>
+  <si>
+    <t>Eu, ADM quero fazer alterações nas permissões dos perfis</t>
+  </si>
+  <si>
+    <t>Eu, ADM quero salvar alterações nas permissões dos perfis</t>
+  </si>
+  <si>
+    <t>Configurar perfil</t>
+  </si>
+  <si>
+    <t>votar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,7 +402,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -432,7 +454,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -626,21 +648,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
@@ -649,12 +671,12 @@
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="D1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
@@ -671,7 +693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -686,7 +708,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -701,7 +723,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
@@ -716,7 +738,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
@@ -731,7 +753,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
@@ -746,7 +768,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
@@ -761,7 +783,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>45</v>
       </c>
@@ -776,7 +798,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
@@ -791,7 +813,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -806,7 +828,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
@@ -821,7 +843,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
@@ -836,7 +858,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
@@ -851,7 +873,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -866,7 +888,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
@@ -881,7 +903,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>43</v>
       </c>
@@ -896,7 +918,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
@@ -911,7 +933,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
         <v>43</v>
       </c>
@@ -926,7 +948,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
@@ -941,7 +963,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
         <v>43</v>
       </c>
@@ -956,7 +978,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
@@ -971,7 +993,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
@@ -986,7 +1008,7 @@
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
@@ -1001,7 +1023,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
@@ -1016,7 +1038,7 @@
       </c>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
         <v>43</v>
       </c>
@@ -1031,7 +1053,7 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
         <v>43</v>
       </c>
@@ -1046,7 +1068,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
@@ -1061,7 +1083,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
         <v>43</v>
       </c>
@@ -1076,7 +1098,7 @@
       </c>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
         <v>44</v>
       </c>
@@ -1091,7 +1113,7 @@
       </c>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -1106,7 +1128,7 @@
       </c>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
@@ -1121,7 +1143,7 @@
       </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -1136,7 +1158,7 @@
       </c>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -1151,7 +1173,7 @@
       </c>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
@@ -1166,7 +1188,7 @@
       </c>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
@@ -1181,7 +1203,7 @@
       </c>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
         <v>44</v>
       </c>
@@ -1195,7 +1217,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
         <v>44</v>
       </c>
@@ -1209,7 +1231,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -1223,7 +1245,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1237,7 +1259,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
         <v>44</v>
       </c>
@@ -1252,7 +1274,7 @@
       </c>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -1267,7 +1289,7 @@
       </c>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -1282,7 +1304,7 @@
       </c>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
@@ -1296,7 +1318,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
@@ -1310,7 +1332,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
         <v>62</v>
@@ -1319,7 +1341,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="7"/>
       <c r="B47" s="2" t="s">
         <v>62</v>
@@ -1328,7 +1350,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
         <v>62</v>
@@ -1337,7 +1359,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
         <v>62</v>
@@ -1346,12 +1368,81 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
-      <c r="C50" s="3"/>
-      <c r="D50">
-        <f>SUM(D3:D49)</f>
-        <v>176</v>
+    <row r="50" spans="1:4">
+      <c r="B50" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="B51" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="B52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="B53" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="B54" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="B55" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="B56" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>